<commit_message>
all scenarios for Add/edit/sort users
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/usertestdata.xlsx
+++ b/src/test/resources/testdata/usertestdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdesh\git\LMS_Hackathon\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151A8165-1196-424D-890C-88943C97402C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DA6066-8CEB-459D-B33A-00856B3B310B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B1C51ABA-3E92-4239-8245-29F0466D1FE3}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="169">
   <si>
     <t>SampleLast</t>
   </si>
@@ -315,12 +315,6 @@
     <t>Mexico</t>
   </si>
   <si>
-    <t>Middle name is required</t>
-  </si>
-  <si>
-    <t>Phone no  is required</t>
-  </si>
-  <si>
     <t>Location is required</t>
   </si>
   <si>
@@ -514,6 +508,36 @@
   </si>
   <si>
     <t>update all text fields special char</t>
+  </si>
+  <si>
+    <t>userdetailsfields</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>user mandatory fields negative</t>
+  </si>
+  <si>
+    <t>Successful</t>
+  </si>
+  <si>
+    <t>1131436526</t>
+  </si>
+  <si>
+    <t>mqgqyrsssb@abc.com</t>
+  </si>
+  <si>
+    <t>Middle name  is required</t>
+  </si>
+  <si>
+    <t>asfd@gmail.com</t>
+  </si>
+  <si>
+    <t>User Role Status is required</t>
+  </si>
+  <si>
+    <t>Phone number  is required</t>
   </si>
 </sst>
 </file>
@@ -963,10 +987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47AA0240-4E7D-4B45-BDDD-9936E80CA8A2}">
-  <dimension ref="A1:S33"/>
+  <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="J10" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1029,13 +1053,13 @@
         <v>40</v>
       </c>
       <c r="Q1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="R1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="S1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
@@ -1043,7 +1067,7 @@
         <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -1052,7 +1076,7 @@
         <v>17</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c r="F2" t="s">
         <v>1</v>
@@ -1076,7 +1100,7 @@
         <v>36</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>31</v>
@@ -1085,15 +1109,15 @@
         <v>30</v>
       </c>
       <c r="P2" t="s">
-        <v>4</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B3">
-        <v>134</v>
+        <v>161</v>
+      </c>
+      <c r="B3" t="s">
+        <v>138</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
@@ -1101,8 +1125,8 @@
       <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="8">
-        <v>1139363260</v>
+      <c r="E3" s="8" t="s">
+        <v>139</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
@@ -1126,7 +1150,7 @@
         <v>36</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>31</v>
@@ -1135,15 +1159,15 @@
         <v>30</v>
       </c>
       <c r="P3" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>136</v>
-      </c>
-      <c r="B4" t="s">
-        <v>137</v>
+        <v>134</v>
+      </c>
+      <c r="B4">
+        <v>134</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
@@ -1176,7 +1200,7 @@
         <v>36</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>31</v>
@@ -1185,15 +1209,15 @@
         <v>30</v>
       </c>
       <c r="P4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
@@ -1226,7 +1250,7 @@
         <v>36</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>31</v>
@@ -1235,15 +1259,15 @@
         <v>30</v>
       </c>
       <c r="P5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" t="s">
         <v>136</v>
-      </c>
-      <c r="B6" t="s">
-        <v>138</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
@@ -1276,7 +1300,7 @@
         <v>36</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>31</v>
@@ -1285,15 +1309,15 @@
         <v>30</v>
       </c>
       <c r="P6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>136</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
@@ -1326,7 +1350,7 @@
         <v>36</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>55</v>
+        <v>131</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>31</v>
@@ -1335,12 +1359,12 @@
         <v>30</v>
       </c>
       <c r="P7" t="s">
-        <v>4</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -1390,7 +1414,10 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>112</v>
+        <v>130</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
@@ -1398,8 +1425,8 @@
       <c r="D9" t="s">
         <v>17</v>
       </c>
-      <c r="E9" t="s">
-        <v>56</v>
+      <c r="E9" s="8">
+        <v>1139363260</v>
       </c>
       <c r="F9" t="s">
         <v>1</v>
@@ -1432,18 +1459,15 @@
         <v>30</v>
       </c>
       <c r="P9" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>122</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>113</v>
-      </c>
-      <c r="B10" t="s">
-        <v>104</v>
+        <v>110</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
@@ -1482,24 +1506,24 @@
         <v>30</v>
       </c>
       <c r="P10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Q10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B11" t="s">
-        <v>106</v>
-      </c>
-      <c r="C11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="8">
-        <v>1234454333</v>
+      <c r="E11" t="s">
+        <v>56</v>
       </c>
       <c r="F11" t="s">
         <v>1</v>
@@ -1532,26 +1556,25 @@
         <v>30</v>
       </c>
       <c r="P11" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="Q11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
       </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="8"/>
+      <c r="E12" s="8">
+        <v>1234454333</v>
+      </c>
       <c r="F12" t="s">
         <v>1</v>
       </c>
@@ -1583,18 +1606,18 @@
         <v>30</v>
       </c>
       <c r="P12" t="s">
-        <v>95</v>
+        <v>165</v>
       </c>
       <c r="Q12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
@@ -1633,18 +1656,18 @@
         <v>30</v>
       </c>
       <c r="P13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="Q13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
@@ -1683,15 +1706,15 @@
         <v>30</v>
       </c>
       <c r="P14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="Q14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
@@ -1734,15 +1757,15 @@
         <v>30</v>
       </c>
       <c r="P15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="Q15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
@@ -1784,15 +1807,15 @@
         <v>30</v>
       </c>
       <c r="P16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="Q16" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
@@ -1834,15 +1857,15 @@
         <v>30</v>
       </c>
       <c r="P17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="Q17" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
@@ -1884,18 +1907,18 @@
         <v>30</v>
       </c>
       <c r="P18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="Q18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>104</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>
@@ -1903,11 +1926,9 @@
       <c r="D19" t="s">
         <v>17</v>
       </c>
-      <c r="E19" t="s">
-        <v>56</v>
-      </c>
+      <c r="E19" s="8"/>
       <c r="F19" t="s">
-        <v>93</v>
+        <v>1</v>
       </c>
       <c r="G19" t="s">
         <v>18</v>
@@ -1921,10 +1942,15 @@
       <c r="J19" t="s">
         <v>21</v>
       </c>
+      <c r="K19" t="s">
+        <v>22</v>
+      </c>
       <c r="L19" t="s">
         <v>36</v>
       </c>
-      <c r="M19" s="1"/>
+      <c r="M19" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="N19" s="1" t="s">
         <v>31</v>
       </c>
@@ -1932,15 +1958,15 @@
         <v>30</v>
       </c>
       <c r="P19" t="s">
-        <v>102</v>
+        <v>168</v>
       </c>
       <c r="Q19" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="B20" t="s">
         <v>16</v>
@@ -1972,9 +1998,10 @@
       <c r="K20" t="s">
         <v>22</v>
       </c>
-      <c r="M20" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="L20" t="s">
+        <v>36</v>
+      </c>
+      <c r="M20" s="1"/>
       <c r="N20" s="1" t="s">
         <v>31</v>
       </c>
@@ -1982,15 +2009,15 @@
         <v>30</v>
       </c>
       <c r="P20" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="Q20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B21" t="s">
         <v>16</v>
@@ -2022,10 +2049,9 @@
       <c r="K21" t="s">
         <v>22</v>
       </c>
-      <c r="L21" t="s">
-        <v>36</v>
-      </c>
-      <c r="M21" s="1"/>
+      <c r="M21" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="N21" s="1" t="s">
         <v>31</v>
       </c>
@@ -2036,24 +2062,27 @@
         <v>101</v>
       </c>
       <c r="Q21" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B22" t="s">
-        <v>105</v>
+        <v>16</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
       </c>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
       <c r="E22" t="s">
         <v>56</v>
       </c>
       <c r="F22" t="s">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="G22" t="s">
         <v>18</v>
@@ -2074,131 +2103,124 @@
         <v>36</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>31</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="N22" s="1"/>
       <c r="O22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="P22" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>89</v>
-      </c>
-      <c r="H23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
+        <v>109</v>
+      </c>
+      <c r="B23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" t="s">
+        <v>22</v>
+      </c>
+      <c r="L23" t="s">
+        <v>36</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P23" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>122</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>134</v>
-      </c>
-      <c r="B24" t="s">
-        <v>140</v>
-      </c>
-      <c r="C24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="F24" t="s">
-        <v>1</v>
-      </c>
-      <c r="G24" t="s">
-        <v>18</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I24" t="s">
-        <v>20</v>
-      </c>
-      <c r="J24" t="s">
-        <v>21</v>
-      </c>
-      <c r="K24" t="s">
-        <v>22</v>
-      </c>
-      <c r="L24" t="s">
-        <v>36</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>142</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="M24" s="1"/>
       <c r="N24" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>30</v>
       </c>
       <c r="P24" t="s">
-        <v>4</v>
+        <v>88</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>135</v>
-      </c>
-      <c r="B25">
-        <v>1111</v>
-      </c>
-      <c r="C25">
-        <v>1111</v>
-      </c>
-      <c r="D25">
-        <v>1111</v>
-      </c>
-      <c r="E25">
-        <v>1139367260</v>
-      </c>
-      <c r="F25">
-        <v>1111</v>
-      </c>
-      <c r="G25">
-        <v>1111</v>
-      </c>
-      <c r="H25" s="1">
-        <v>1111</v>
-      </c>
-      <c r="I25">
-        <v>111</v>
-      </c>
-      <c r="J25">
-        <v>111</v>
-      </c>
-      <c r="K25">
-        <v>111</v>
-      </c>
-      <c r="L25">
-        <v>111</v>
-      </c>
-      <c r="M25" s="1">
-        <v>111</v>
-      </c>
-      <c r="N25" s="1">
-        <v>111</v>
-      </c>
-      <c r="O25" s="1">
-        <v>111</v>
+        <v>132</v>
+      </c>
+      <c r="B25" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J25" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25" t="s">
+        <v>22</v>
+      </c>
+      <c r="L25" t="s">
+        <v>36</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="P25" t="s">
         <v>4</v>
@@ -2206,106 +2228,119 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>145</v>
-      </c>
-      <c r="B26" t="s">
-        <v>140</v>
-      </c>
-      <c r="C26" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="F26" t="s">
-        <v>1</v>
-      </c>
-      <c r="G26" t="s">
-        <v>18</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I26" t="s">
-        <v>20</v>
-      </c>
-      <c r="J26" t="s">
-        <v>21</v>
-      </c>
-      <c r="K26" t="s">
-        <v>22</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" t="s">
-        <v>144</v>
+        <v>133</v>
+      </c>
+      <c r="B26">
+        <v>1111</v>
+      </c>
+      <c r="C26">
+        <v>1111</v>
+      </c>
+      <c r="D26">
+        <v>1111</v>
+      </c>
+      <c r="E26">
+        <v>1139367260</v>
+      </c>
+      <c r="F26">
+        <v>1111</v>
+      </c>
+      <c r="G26">
+        <v>1111</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1111</v>
+      </c>
+      <c r="I26">
+        <v>111</v>
+      </c>
+      <c r="J26">
+        <v>111</v>
+      </c>
+      <c r="K26">
+        <v>111</v>
+      </c>
+      <c r="L26">
+        <v>111</v>
+      </c>
+      <c r="M26" s="1">
+        <v>111</v>
+      </c>
+      <c r="N26" s="1">
+        <v>111</v>
+      </c>
+      <c r="O26" s="1">
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>147</v>
-      </c>
-      <c r="D27" t="s">
-        <v>146</v>
-      </c>
-      <c r="E27" s="8"/>
-      <c r="H27" s="1"/>
+        <v>143</v>
+      </c>
+      <c r="B27" t="s">
+        <v>138</v>
+      </c>
+      <c r="C27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J27" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" t="s">
+        <v>22</v>
+      </c>
+      <c r="L27" t="s">
+        <v>36</v>
+      </c>
       <c r="M27" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P27" t="s">
         <v>142</v>
-      </c>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="P27" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>123</v>
-      </c>
-      <c r="B28" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" t="s">
-        <v>61</v>
+        <v>145</v>
       </c>
       <c r="D28" t="s">
-        <v>62</v>
-      </c>
-      <c r="E28" t="s">
-        <v>63</v>
-      </c>
-      <c r="F28" t="s">
-        <v>64</v>
-      </c>
-      <c r="G28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H28" t="s">
-        <v>71</v>
-      </c>
-      <c r="I28" t="s">
-        <v>66</v>
-      </c>
-      <c r="J28" t="s">
-        <v>67</v>
-      </c>
-      <c r="K28" t="s">
-        <v>68</v>
-      </c>
-      <c r="L28" t="s">
-        <v>87</v>
-      </c>
-      <c r="M28" t="s">
-        <v>72</v>
+        <v>144</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="H28" s="1"/>
+      <c r="M28" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>128</v>
+        <v>159</v>
       </c>
       <c r="B29" t="s">
         <v>60</v>
@@ -2340,8 +2375,8 @@
       <c r="L29" t="s">
         <v>87</v>
       </c>
-      <c r="M29" s="1" t="s">
-        <v>143</v>
+      <c r="M29" t="s">
+        <v>72</v>
       </c>
       <c r="N29" t="s">
         <v>69</v>
@@ -2349,9 +2384,6 @@
       <c r="O29" t="s">
         <v>70</v>
       </c>
-      <c r="P29" t="s">
-        <v>144</v>
-      </c>
       <c r="R29" t="s">
         <v>124</v>
       </c>
@@ -2361,128 +2393,225 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>148</v>
-      </c>
-      <c r="B30">
-        <v>2222</v>
-      </c>
-      <c r="C30">
-        <v>1222</v>
-      </c>
-      <c r="D30">
-        <v>2222</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F30">
-        <v>111</v>
-      </c>
-      <c r="G30">
-        <v>111</v>
-      </c>
-      <c r="H30" s="1">
-        <v>111</v>
-      </c>
-      <c r="I30">
-        <v>11</v>
-      </c>
-      <c r="J30">
-        <v>11</v>
-      </c>
-      <c r="K30">
-        <v>111</v>
-      </c>
-      <c r="L30">
-        <v>111</v>
-      </c>
-      <c r="M30" s="1">
-        <v>1111</v>
-      </c>
-      <c r="N30" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O30" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P30" t="s">
-        <v>150</v>
+        <v>121</v>
+      </c>
+      <c r="B30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G30" t="s">
+        <v>65</v>
+      </c>
+      <c r="H30" t="s">
+        <v>71</v>
+      </c>
+      <c r="I30" t="s">
+        <v>66</v>
+      </c>
+      <c r="J30" t="s">
+        <v>67</v>
+      </c>
+      <c r="K30" t="s">
+        <v>68</v>
+      </c>
+      <c r="L30" t="s">
+        <v>87</v>
+      </c>
+      <c r="M30" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>160</v>
+        <v>126</v>
       </c>
       <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" t="s">
+        <v>63</v>
+      </c>
+      <c r="F31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G31" t="s">
+        <v>65</v>
+      </c>
+      <c r="H31" t="s">
+        <v>71</v>
+      </c>
+      <c r="I31" t="s">
+        <v>66</v>
+      </c>
+      <c r="J31" t="s">
+        <v>67</v>
+      </c>
+      <c r="K31" t="s">
+        <v>68</v>
+      </c>
+      <c r="L31" t="s">
+        <v>87</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="N31" t="s">
+        <v>69</v>
+      </c>
+      <c r="O31" t="s">
+        <v>70</v>
+      </c>
+      <c r="P31" t="s">
+        <v>142</v>
+      </c>
+      <c r="R31" t="s">
+        <v>122</v>
+      </c>
+      <c r="S31" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>146</v>
+      </c>
+      <c r="B32">
+        <v>2222</v>
+      </c>
+      <c r="C32">
+        <v>1222</v>
+      </c>
+      <c r="D32">
+        <v>2222</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="F32">
+        <v>111</v>
+      </c>
+      <c r="G32">
+        <v>111</v>
+      </c>
+      <c r="H32" s="1">
+        <v>111</v>
+      </c>
+      <c r="I32">
+        <v>11</v>
+      </c>
+      <c r="J32">
+        <v>11</v>
+      </c>
+      <c r="K32">
+        <v>111</v>
+      </c>
+      <c r="L32">
+        <v>111</v>
+      </c>
+      <c r="M32" s="1">
+        <v>1111</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P32" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>158</v>
+      </c>
+      <c r="B33" t="s">
+        <v>149</v>
+      </c>
+      <c r="C33" t="s">
+        <v>149</v>
+      </c>
+      <c r="D33" t="s">
+        <v>150</v>
+      </c>
+      <c r="E33" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="C31" t="s">
-        <v>151</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="F33" t="s">
+        <v>135</v>
+      </c>
+      <c r="G33" t="s">
         <v>152</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="H33" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F31" t="s">
-        <v>137</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="I33" t="s">
         <v>154</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="J33" t="s">
         <v>155</v>
       </c>
-      <c r="I31" t="s">
+      <c r="K33" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="J31" t="s">
+      <c r="L33" t="s">
         <v>157</v>
       </c>
-      <c r="K31" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="L31" t="s">
-        <v>159</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="N31" s="1" t="s">
+      <c r="M33" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="N33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O31" s="1" t="s">
+      <c r="O33" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="P31" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A32" s="9"/>
-      <c r="H32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-    </row>
-    <row r="33" spans="13:15" x14ac:dyDescent="0.35">
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
+      <c r="P33" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A34" s="9"/>
+      <c r="H34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="M2" r:id="rId1" xr:uid="{40159C53-F4E6-4203-9253-F0A8D36FA8E6}"/>
-    <hyperlink ref="M33" r:id="rId2" display="sample9@sample.com" xr:uid="{0BF1F079-FE55-4017-A95F-D160A11F5B5D}"/>
+    <hyperlink ref="M35" r:id="rId2" display="sample9@sample.com" xr:uid="{0BF1F079-FE55-4017-A95F-D160A11F5B5D}"/>
     <hyperlink ref="H2" r:id="rId3" xr:uid="{571EDCCE-FC5B-417C-AA30-F32CE06CAC18}"/>
-    <hyperlink ref="M10" r:id="rId4" xr:uid="{8B235457-3B83-4BB9-9B00-E6D0E86A1320}"/>
-    <hyperlink ref="H10" r:id="rId5" xr:uid="{D8F0CB93-48C6-40C0-B6E6-107726CD1108}"/>
-    <hyperlink ref="M22" r:id="rId6" xr:uid="{EA4E4C74-534C-485F-9D84-3381E51209B1}"/>
-    <hyperlink ref="H22" r:id="rId7" xr:uid="{B7C96E4F-5A91-4CAA-89B2-1EF3AEFECCF7}"/>
-    <hyperlink ref="M11" r:id="rId8" xr:uid="{97433741-1138-464C-905E-4C3B2163CE26}"/>
-    <hyperlink ref="H11" r:id="rId9" xr:uid="{09A84E83-52C8-442A-B053-EDF7B3D6C1D8}"/>
+    <hyperlink ref="M11" r:id="rId4" xr:uid="{8B235457-3B83-4BB9-9B00-E6D0E86A1320}"/>
+    <hyperlink ref="H11" r:id="rId5" xr:uid="{D8F0CB93-48C6-40C0-B6E6-107726CD1108}"/>
+    <hyperlink ref="M23" r:id="rId6" xr:uid="{EA4E4C74-534C-485F-9D84-3381E51209B1}"/>
+    <hyperlink ref="H23" r:id="rId7" xr:uid="{B7C96E4F-5A91-4CAA-89B2-1EF3AEFECCF7}"/>
+    <hyperlink ref="M12" r:id="rId8" xr:uid="{97433741-1138-464C-905E-4C3B2163CE26}"/>
+    <hyperlink ref="H12" r:id="rId9" xr:uid="{09A84E83-52C8-442A-B053-EDF7B3D6C1D8}"/>
     <hyperlink ref="M13" r:id="rId10" xr:uid="{39271BC9-C23E-4EA9-8884-127AC0D704FB}"/>
     <hyperlink ref="H13" r:id="rId11" xr:uid="{6A7B3276-1AF1-4BB7-BF9F-D574165A15A5}"/>
     <hyperlink ref="M14" r:id="rId12" xr:uid="{D9A4845A-FCB6-406D-AE9D-9A5A4AE9632D}"/>
@@ -2490,43 +2619,46 @@
     <hyperlink ref="M16" r:id="rId14" xr:uid="{49E4F761-7624-4B87-910C-A092C376BD50}"/>
     <hyperlink ref="M17" r:id="rId15" xr:uid="{265FCA21-CF44-45A7-AB36-5FC716B78B2A}"/>
     <hyperlink ref="M18" r:id="rId16" xr:uid="{1BAA0765-A95E-4FBB-923B-0C474D4B206C}"/>
-    <hyperlink ref="M20" r:id="rId17" xr:uid="{D984BA1D-5060-453D-AAD9-9B2E43FD6E32}"/>
+    <hyperlink ref="M21" r:id="rId17" xr:uid="{D984BA1D-5060-453D-AAD9-9B2E43FD6E32}"/>
     <hyperlink ref="H14" r:id="rId18" xr:uid="{FFA70586-3912-4CF9-81E7-9A668E324D66}"/>
     <hyperlink ref="H16" r:id="rId19" xr:uid="{74FD5586-F678-4AD5-938D-E90B11661EBF}"/>
     <hyperlink ref="H17" r:id="rId20" xr:uid="{8FAE19CF-9215-4BD2-B27E-A95CB040C825}"/>
     <hyperlink ref="H18" r:id="rId21" xr:uid="{873DA314-7B0B-4E93-A687-4E43E6BEE8A4}"/>
-    <hyperlink ref="H20" r:id="rId22" xr:uid="{70BB04AC-10A3-42DC-97AF-7885BCE9601E}"/>
-    <hyperlink ref="H21" r:id="rId23" xr:uid="{04FE1C3C-468D-44B9-9F53-836087EC0644}"/>
-    <hyperlink ref="M12" r:id="rId24" xr:uid="{1D2197E0-270A-499E-A9BA-A6ED6455C7A0}"/>
-    <hyperlink ref="H12" r:id="rId25" xr:uid="{42A73A6E-B523-4023-846C-C60B7BE875B5}"/>
-    <hyperlink ref="H19" r:id="rId26" xr:uid="{E0776F6A-68CD-46AA-AD9D-149F03C5B37D}"/>
-    <hyperlink ref="H9" r:id="rId27" xr:uid="{C6E8536B-2300-445E-83A7-C82705F5ABBE}"/>
-    <hyperlink ref="M9" r:id="rId28" xr:uid="{CD418853-C9E8-40FA-8129-A630E1678CFF}"/>
-    <hyperlink ref="M7" r:id="rId29" xr:uid="{61B39585-7390-4CD8-8077-266C11A755C1}"/>
-    <hyperlink ref="H7" r:id="rId30" xr:uid="{7EB8E70E-9F4A-46C4-ACDF-4BCEDB996546}"/>
-    <hyperlink ref="M8" r:id="rId31" xr:uid="{3A91BAC8-F096-4376-894E-83066DFB4349}"/>
-    <hyperlink ref="H8" r:id="rId32" xr:uid="{456D4A44-38F7-481B-B72A-96D201DFFA86}"/>
-    <hyperlink ref="M25" r:id="rId33" display="aqdgsseb@abc.com" xr:uid="{4FAA7EC7-8DD1-4FF2-ADA0-EB0ACF536EA7}"/>
-    <hyperlink ref="H25" r:id="rId34" display="www.linkedin.com/team2" xr:uid="{E97FCEDD-009E-4842-B1E6-016BDEC1276B}"/>
-    <hyperlink ref="M3" r:id="rId35" xr:uid="{F70BE9D9-139C-4FAD-9C5D-B35F1B032D3D}"/>
-    <hyperlink ref="H3" r:id="rId36" xr:uid="{E46B6720-4EEB-455D-AEE1-9D9B539F4F46}"/>
-    <hyperlink ref="M4" r:id="rId37" xr:uid="{EF982342-133C-4044-8FA5-DD21A3BE43FD}"/>
-    <hyperlink ref="H4" r:id="rId38" xr:uid="{92BF9005-D879-43EB-AAAD-D6FC6BBACCA2}"/>
-    <hyperlink ref="M5" r:id="rId39" xr:uid="{24A061BA-78E3-49A9-B4EC-CAF49932DD2A}"/>
-    <hyperlink ref="H5" r:id="rId40" xr:uid="{7ABCF620-8DAD-4E9B-9069-5B9CFE8CD453}"/>
-    <hyperlink ref="M6" r:id="rId41" xr:uid="{3DD837E5-D1C8-4646-BFAC-BA3CEC2EBF16}"/>
-    <hyperlink ref="H6" r:id="rId42" xr:uid="{32447EA6-AE70-4ADE-A8B1-3FFB72E45A63}"/>
-    <hyperlink ref="M24" r:id="rId43" xr:uid="{9851D807-AF6E-4826-8D08-4AD494133184}"/>
-    <hyperlink ref="H24" r:id="rId44" xr:uid="{81045F02-1CC8-4416-A1F8-93691D6759FF}"/>
-    <hyperlink ref="M29" r:id="rId45" xr:uid="{DCEEDA8E-0245-4855-B8B8-6EAD0B1CD640}"/>
-    <hyperlink ref="M26" r:id="rId46" xr:uid="{2EBBE650-CA71-4627-8727-D87E3FE6AC61}"/>
-    <hyperlink ref="H26" r:id="rId47" xr:uid="{954CB31D-4B30-4968-A859-415AEC1F574C}"/>
-    <hyperlink ref="M27" r:id="rId48" xr:uid="{403668BD-AD7B-4C5C-A9A6-8F5D4002C10C}"/>
-    <hyperlink ref="M30" r:id="rId49" display="aqdgqsssb@abc.com" xr:uid="{03944273-872B-46D4-A83C-B0E1D1139F0F}"/>
-    <hyperlink ref="H30" r:id="rId50" display="www.linkedin.com/team2" xr:uid="{775452D3-6DDC-423C-BC7B-EEE28B5B20F2}"/>
-    <hyperlink ref="M31" r:id="rId51" display="aqdgqsssb@abc.com" xr:uid="{0743A2B7-4766-4342-B148-9E34344122D1}"/>
-    <hyperlink ref="H31" r:id="rId52" display="www.linkedin.com/team2" xr:uid="{C0E926E2-9DA4-4A32-894C-E936092348D6}"/>
-    <hyperlink ref="K31" r:id="rId53" xr:uid="{5249AABA-1D56-4CD6-9C74-D94E0FA4E4D9}"/>
+    <hyperlink ref="H21" r:id="rId22" xr:uid="{70BB04AC-10A3-42DC-97AF-7885BCE9601E}"/>
+    <hyperlink ref="H22" r:id="rId23" xr:uid="{04FE1C3C-468D-44B9-9F53-836087EC0644}"/>
+    <hyperlink ref="M19" r:id="rId24" xr:uid="{1D2197E0-270A-499E-A9BA-A6ED6455C7A0}"/>
+    <hyperlink ref="H19" r:id="rId25" xr:uid="{42A73A6E-B523-4023-846C-C60B7BE875B5}"/>
+    <hyperlink ref="H20" r:id="rId26" xr:uid="{E0776F6A-68CD-46AA-AD9D-149F03C5B37D}"/>
+    <hyperlink ref="H10" r:id="rId27" xr:uid="{C6E8536B-2300-445E-83A7-C82705F5ABBE}"/>
+    <hyperlink ref="M10" r:id="rId28" xr:uid="{CD418853-C9E8-40FA-8129-A630E1678CFF}"/>
+    <hyperlink ref="M8" r:id="rId29" xr:uid="{61B39585-7390-4CD8-8077-266C11A755C1}"/>
+    <hyperlink ref="H8" r:id="rId30" xr:uid="{7EB8E70E-9F4A-46C4-ACDF-4BCEDB996546}"/>
+    <hyperlink ref="M9" r:id="rId31" xr:uid="{3A91BAC8-F096-4376-894E-83066DFB4349}"/>
+    <hyperlink ref="H9" r:id="rId32" xr:uid="{456D4A44-38F7-481B-B72A-96D201DFFA86}"/>
+    <hyperlink ref="M26" r:id="rId33" display="aqdgsseb@abc.com" xr:uid="{4FAA7EC7-8DD1-4FF2-ADA0-EB0ACF536EA7}"/>
+    <hyperlink ref="H26" r:id="rId34" display="www.linkedin.com/team2" xr:uid="{E97FCEDD-009E-4842-B1E6-016BDEC1276B}"/>
+    <hyperlink ref="M4" r:id="rId35" xr:uid="{F70BE9D9-139C-4FAD-9C5D-B35F1B032D3D}"/>
+    <hyperlink ref="H4" r:id="rId36" xr:uid="{E46B6720-4EEB-455D-AEE1-9D9B539F4F46}"/>
+    <hyperlink ref="M5" r:id="rId37" xr:uid="{EF982342-133C-4044-8FA5-DD21A3BE43FD}"/>
+    <hyperlink ref="H5" r:id="rId38" xr:uid="{92BF9005-D879-43EB-AAAD-D6FC6BBACCA2}"/>
+    <hyperlink ref="M6" r:id="rId39" xr:uid="{24A061BA-78E3-49A9-B4EC-CAF49932DD2A}"/>
+    <hyperlink ref="H6" r:id="rId40" xr:uid="{7ABCF620-8DAD-4E9B-9069-5B9CFE8CD453}"/>
+    <hyperlink ref="M7" r:id="rId41" xr:uid="{3DD837E5-D1C8-4646-BFAC-BA3CEC2EBF16}"/>
+    <hyperlink ref="H7" r:id="rId42" xr:uid="{32447EA6-AE70-4ADE-A8B1-3FFB72E45A63}"/>
+    <hyperlink ref="M25" r:id="rId43" xr:uid="{9851D807-AF6E-4826-8D08-4AD494133184}"/>
+    <hyperlink ref="H25" r:id="rId44" xr:uid="{81045F02-1CC8-4416-A1F8-93691D6759FF}"/>
+    <hyperlink ref="M31" r:id="rId45" xr:uid="{DCEEDA8E-0245-4855-B8B8-6EAD0B1CD640}"/>
+    <hyperlink ref="M27" r:id="rId46" xr:uid="{2EBBE650-CA71-4627-8727-D87E3FE6AC61}"/>
+    <hyperlink ref="H27" r:id="rId47" xr:uid="{954CB31D-4B30-4968-A859-415AEC1F574C}"/>
+    <hyperlink ref="M28" r:id="rId48" xr:uid="{403668BD-AD7B-4C5C-A9A6-8F5D4002C10C}"/>
+    <hyperlink ref="M32" r:id="rId49" display="aqdgqsssb@abc.com" xr:uid="{03944273-872B-46D4-A83C-B0E1D1139F0F}"/>
+    <hyperlink ref="H32" r:id="rId50" display="www.linkedin.com/team2" xr:uid="{775452D3-6DDC-423C-BC7B-EEE28B5B20F2}"/>
+    <hyperlink ref="M33" r:id="rId51" display="aqdgqsssb@abc.com" xr:uid="{0743A2B7-4766-4342-B148-9E34344122D1}"/>
+    <hyperlink ref="H33" r:id="rId52" display="www.linkedin.com/team2" xr:uid="{C0E926E2-9DA4-4A32-894C-E936092348D6}"/>
+    <hyperlink ref="K33" r:id="rId53" xr:uid="{5249AABA-1D56-4CD6-9C74-D94E0FA4E4D9}"/>
+    <hyperlink ref="M3" r:id="rId54" xr:uid="{DCBBA3BA-4A3F-4E0B-AFEB-83D316100431}"/>
+    <hyperlink ref="H3" r:id="rId55" xr:uid="{9290C624-B549-4276-88E5-B8B1EE5BEB82}"/>
+    <hyperlink ref="M22" r:id="rId56" xr:uid="{489A1CB0-5631-463C-9DB2-1929CBF87357}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>